<commit_message>
keshavarzi bank is done
</commit_message>
<xml_diff>
--- a/Asgari_Tasks/Iranian_Banks_Data/Iranian_Banks.xlsx
+++ b/Asgari_Tasks/Iranian_Banks_Data/Iranian_Banks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A2F415-E14C-4601-BAE7-C41A5F833C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C169BDB9-C70E-44E2-85C0-B2644FA4807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t>Bank Name</t>
   </si>
@@ -323,6 +323,27 @@
   </si>
   <si>
     <t>resalat_bank_branches_20241103</t>
+  </si>
+  <si>
+    <t>mehreiranian_bank_branches_20241105</t>
+  </si>
+  <si>
+    <t>toseesaderat_bank_branches_20241113</t>
+  </si>
+  <si>
+    <t>khavarmianeh_bank_branches_20241115</t>
+  </si>
+  <si>
+    <t>iranzamin_bank_branches_20241117</t>
+  </si>
+  <si>
+    <t>sina_bank_branches_20241117</t>
+  </si>
+  <si>
+    <t>saman_bank_branches_20241119</t>
+  </si>
+  <si>
+    <t>keshavarzi_bank_branches_20241120</t>
   </si>
 </sst>
 </file>
@@ -343,7 +364,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +374,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,19 +411,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -695,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,6 +830,9 @@
       <c r="C6" t="s">
         <v>60</v>
       </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
       <c r="E6" t="s">
         <v>65</v>
       </c>
@@ -819,29 +855,30 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -908,17 +945,17 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -930,38 +967,44 @@
       <c r="C15" t="s">
         <v>60</v>
       </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
       <c r="E15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1026,7 +1069,9 @@
       <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
       <c r="E21" t="s">
         <v>86</v>
       </c>
@@ -1049,19 +1094,19 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1075,22 +1120,27 @@
       <c r="C24" t="s">
         <v>60</v>
       </c>
+      <c r="D24" t="s">
+        <v>104</v>
+      </c>
       <c r="E24" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1112,34 +1162,36 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2" t="s">
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>